<commit_message>
feat: automatic drive upload on update and download links
</commit_message>
<xml_diff>
--- a/crypto_data.xlsx
+++ b/crypto_data.xlsx
@@ -494,19 +494,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98081.08</v>
+        <v>97723.44</v>
       </c>
       <c r="D2" t="n">
-        <v>1492239705.894488</v>
+        <v>1493445441.35651</v>
       </c>
       <c r="E2" t="n">
-        <v>15214.34823</v>
+        <v>15282.36666</v>
       </c>
       <c r="F2" t="n">
-        <v>0.326</v>
+        <v>0.354</v>
       </c>
       <c r="G2" t="n">
-        <v>97679.06132084</v>
+        <v>97689.78722031999</v>
       </c>
     </row>
     <row r="3">
@@ -521,19 +521,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2700.98</v>
+        <v>2685.93</v>
       </c>
       <c r="D3" t="n">
-        <v>998531753.432886</v>
+        <v>997614352.494786</v>
       </c>
       <c r="E3" t="n">
-        <v>369692.3907</v>
+        <v>371422.3202</v>
       </c>
       <c r="F3" t="n">
-        <v>2.108</v>
+        <v>1.582</v>
       </c>
       <c r="G3" t="n">
-        <v>2682.71216057</v>
+        <v>2684.33109043</v>
       </c>
     </row>
     <row r="4">
@@ -548,19 +548,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9998</v>
+        <v>0.9997</v>
       </c>
       <c r="D4" t="n">
-        <v>866381902.9572001</v>
+        <v>902809385.9070001</v>
       </c>
       <c r="E4" t="n">
-        <v>866555214</v>
+        <v>903080310</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="G4" t="n">
-        <v>0.99982609</v>
+        <v>0.99982084</v>
       </c>
     </row>
     <row r="5">
@@ -575,19 +575,19 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>202.87</v>
+        <v>201.89</v>
       </c>
       <c r="D5" t="n">
-        <v>849431029.66308</v>
+        <v>857313077.70407</v>
       </c>
       <c r="E5" t="n">
-        <v>4187070.684</v>
+        <v>4246436.563</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.681</v>
+        <v>-0.694</v>
       </c>
       <c r="G5" t="n">
-        <v>203.5476258</v>
+        <v>203.48269591</v>
       </c>
     </row>
     <row r="6">
@@ -602,19 +602,19 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9992</v>
+        <v>0.9991</v>
       </c>
       <c r="D6" t="n">
-        <v>503295684.0856</v>
+        <v>511622726.7582</v>
       </c>
       <c r="E6" t="n">
-        <v>503698643</v>
+        <v>512083602</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="G6" t="n">
-        <v>0.99912923</v>
+        <v>0.99913401</v>
       </c>
     </row>
     <row r="7">
@@ -629,19 +629,19 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2.4879</v>
+        <v>2.4785</v>
       </c>
       <c r="D7" t="n">
-        <v>493973774.0225999</v>
+        <v>493634861.7515</v>
       </c>
       <c r="E7" t="n">
-        <v>198550494</v>
+        <v>199166779</v>
       </c>
       <c r="F7" t="n">
-        <v>2.912</v>
+        <v>2.6</v>
       </c>
       <c r="G7" t="n">
-        <v>2.46202943</v>
+        <v>2.46397955</v>
       </c>
     </row>
     <row r="8">
@@ -656,19 +656,19 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.2157</v>
+        <v>0.2117</v>
       </c>
       <c r="D8" t="n">
-        <v>372996254.66001</v>
+        <v>352624169.23118</v>
       </c>
       <c r="E8" t="n">
-        <v>1729236229.3</v>
+        <v>1665678645.4</v>
       </c>
       <c r="F8" t="n">
-        <v>38.358</v>
+        <v>33.48</v>
       </c>
       <c r="G8" t="n">
-        <v>0.19254142</v>
+        <v>0.19521403</v>
       </c>
     </row>
     <row r="9">
@@ -683,19 +683,19 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>128.07</v>
+        <v>129.53</v>
       </c>
       <c r="D9" t="n">
-        <v>301930709.64309</v>
+        <v>292963475.06733</v>
       </c>
       <c r="E9" t="n">
-        <v>2357544.387</v>
+        <v>2261742.261</v>
       </c>
       <c r="F9" t="n">
-        <v>10.845</v>
+        <v>11.051</v>
       </c>
       <c r="G9" t="n">
-        <v>123.61225629</v>
+        <v>124.17140339</v>
       </c>
     </row>
     <row r="10">
@@ -710,19 +710,19 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3.5363</v>
+        <v>3.467</v>
       </c>
       <c r="D10" t="n">
-        <v>288978565.25709</v>
+        <v>286232556.4084</v>
       </c>
       <c r="E10" t="n">
-        <v>81717774.3</v>
+        <v>82559145.2</v>
       </c>
       <c r="F10" t="n">
-        <v>9.483000000000001</v>
+        <v>8.378</v>
       </c>
       <c r="G10" t="n">
-        <v>3.35141646</v>
+        <v>3.36503685</v>
       </c>
     </row>
     <row r="11">
@@ -737,19 +737,19 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>640.12</v>
+        <v>638.64</v>
       </c>
       <c r="D11" t="n">
-        <v>261141234.48244</v>
+        <v>263555275.90752</v>
       </c>
       <c r="E11" t="n">
-        <v>407956.687</v>
+        <v>412682.068</v>
       </c>
       <c r="F11" t="n">
-        <v>5.931</v>
+        <v>5.625</v>
       </c>
       <c r="G11" t="n">
-        <v>624.56412742</v>
+        <v>626.13867103</v>
       </c>
     </row>
     <row r="12">
@@ -764,19 +764,19 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.26503</v>
+        <v>0.26276</v>
       </c>
       <c r="D12" t="n">
-        <v>233085383.10263</v>
+        <v>236436550.27368</v>
       </c>
       <c r="E12" t="n">
-        <v>879467921</v>
+        <v>899819418</v>
       </c>
       <c r="F12" t="n">
-        <v>5.691</v>
+        <v>5.121</v>
       </c>
       <c r="G12" t="n">
-        <v>0.25914745</v>
+        <v>0.25954777</v>
       </c>
     </row>
     <row r="13">
@@ -791,19 +791,19 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.6808999999999999</v>
+        <v>0.6788</v>
       </c>
       <c r="D13" t="n">
-        <v>219863931.83117</v>
+        <v>225714302.71512</v>
       </c>
       <c r="E13" t="n">
-        <v>322901941.3</v>
+        <v>332519597.4</v>
       </c>
       <c r="F13" t="n">
-        <v>24.913</v>
+        <v>35.3</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6534747</v>
+        <v>0.66187316</v>
       </c>
     </row>
     <row r="14">
@@ -818,19 +818,19 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1.033e-05</v>
+        <v>1.023e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>215491091.4939882</v>
+        <v>219520535.6558877</v>
       </c>
       <c r="E14" t="n">
-        <v>20860705856146</v>
+        <v>21458507884251</v>
       </c>
       <c r="F14" t="n">
-        <v>7.941</v>
+        <v>7.458</v>
       </c>
       <c r="G14" t="n">
-        <v>9.96e-06</v>
+        <v>9.989999999999999e-06</v>
       </c>
     </row>
     <row r="15">
@@ -845,19 +845,19 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.8001</v>
+        <v>0.8053</v>
       </c>
       <c r="D15" t="n">
-        <v>220189414.23675</v>
+        <v>226602279.12023</v>
       </c>
       <c r="E15" t="n">
-        <v>275202367.5</v>
+        <v>281388649.1</v>
       </c>
       <c r="F15" t="n">
-        <v>14.464</v>
+        <v>15.555</v>
       </c>
       <c r="G15" t="n">
-        <v>0.75423157</v>
+        <v>0.75739919</v>
       </c>
     </row>
     <row r="16">
@@ -872,19 +872,19 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>16.15</v>
+        <v>15.88</v>
       </c>
       <c r="D16" t="n">
-        <v>187323628.95495</v>
+        <v>188823230.26852</v>
       </c>
       <c r="E16" t="n">
-        <v>11598986.313</v>
+        <v>11890631.629</v>
       </c>
       <c r="F16" t="n">
-        <v>0.623</v>
+        <v>-0.626</v>
       </c>
       <c r="G16" t="n">
-        <v>16.22378641</v>
+        <v>16.21612462</v>
       </c>
     </row>
     <row r="17">
@@ -902,16 +902,16 @@
         <v>0.2482</v>
       </c>
       <c r="D17" t="n">
-        <v>121018042.69494</v>
+        <v>125586081.88822</v>
       </c>
       <c r="E17" t="n">
-        <v>487582766.7</v>
+        <v>505987437.1</v>
       </c>
       <c r="F17" t="n">
-        <v>4.505</v>
+        <v>4.023</v>
       </c>
       <c r="G17" t="n">
-        <v>0.24352706</v>
+        <v>0.24399162</v>
       </c>
     </row>
     <row r="18">
@@ -926,19 +926,19 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.4851</v>
+        <v>0.4754</v>
       </c>
       <c r="D18" t="n">
-        <v>104124529.643904</v>
+        <v>103706108.550178</v>
       </c>
       <c r="E18" t="n">
-        <v>214645495.04</v>
+        <v>218144948.57</v>
       </c>
       <c r="F18" t="n">
-        <v>1.358</v>
+        <v>-0.979</v>
       </c>
       <c r="G18" t="n">
-        <v>0.48823639</v>
+        <v>0.48801697</v>
       </c>
     </row>
     <row r="19">
@@ -953,19 +953,19 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.2851</v>
+        <v>0.2847</v>
       </c>
       <c r="D19" t="n">
-        <v>99267022.99293001</v>
+        <v>98308574.18538</v>
       </c>
       <c r="E19" t="n">
-        <v>348183174.3</v>
+        <v>345305845.4</v>
       </c>
       <c r="F19" t="n">
-        <v>9.108000000000001</v>
+        <v>11.081</v>
       </c>
       <c r="G19" t="n">
-        <v>0.28600563</v>
+        <v>0.28683605</v>
       </c>
     </row>
     <row r="20">
@@ -980,19 +980,19 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1.311</v>
+        <v>1.299</v>
       </c>
       <c r="D20" t="n">
-        <v>90142310.38259999</v>
+        <v>86860919.3916</v>
       </c>
       <c r="E20" t="n">
-        <v>68758436.59999999</v>
+        <v>66867528.4</v>
       </c>
       <c r="F20" t="n">
-        <v>2.985</v>
+        <v>2.203</v>
       </c>
       <c r="G20" t="n">
-        <v>1.29996434</v>
+        <v>1.30058832</v>
       </c>
     </row>
     <row r="21">
@@ -1007,127 +1007,127 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.001071</v>
+        <v>0.001093</v>
       </c>
       <c r="D21" t="n">
-        <v>85140100.18955699</v>
+        <v>90251814.62160499</v>
       </c>
       <c r="E21" t="n">
-        <v>79495891867</v>
+        <v>82572565985</v>
       </c>
       <c r="F21" t="n">
-        <v>54.993</v>
+        <v>61.686</v>
       </c>
       <c r="G21" t="n">
-        <v>0.00095739</v>
+        <v>0.00096763</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Berachain</t>
+          <t>The Anthropic Order</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BERA</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>5.722</v>
+        <v>421.2</v>
       </c>
       <c r="D22" t="n">
-        <v>77193544.921506</v>
+        <v>79876419.63912</v>
       </c>
       <c r="E22" t="n">
-        <v>13490657.973</v>
+        <v>189640.1226</v>
       </c>
       <c r="F22" t="n">
-        <v>14.303</v>
+        <v>8.305</v>
       </c>
       <c r="G22" t="n">
-        <v>5.56015889</v>
+        <v>408.1307934</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>The Anthropic Order</t>
+          <t>Berachain</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>BERA</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>430.2</v>
+        <v>5.57</v>
       </c>
       <c r="D23" t="n">
-        <v>78723118.43442</v>
+        <v>74940461.82808</v>
       </c>
       <c r="E23" t="n">
-        <v>182991.9071</v>
+        <v>13454301.944</v>
       </c>
       <c r="F23" t="n">
-        <v>10.848</v>
+        <v>11.892</v>
       </c>
       <c r="G23" t="n">
-        <v>406.67995057</v>
+        <v>5.58017001</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>THORChain</t>
+          <t>PancakeSwap</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>RUNE</t>
+          <t>CAKE</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1.425</v>
+        <v>1.978</v>
       </c>
       <c r="D24" t="n">
-        <v>73176573.495</v>
+        <v>78365790.83514</v>
       </c>
       <c r="E24" t="n">
-        <v>51351981.4</v>
+        <v>39618701.13</v>
       </c>
       <c r="F24" t="n">
-        <v>6.742</v>
+        <v>19.444</v>
       </c>
       <c r="G24" t="n">
-        <v>1.41220971</v>
+        <v>1.89254516</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PancakeSwap</t>
+          <t>Aptos</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>CAKE</t>
+          <t>APT</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2.03</v>
+        <v>6.08</v>
       </c>
       <c r="D25" t="n">
-        <v>77884912.86449999</v>
+        <v>68274945.04000001</v>
       </c>
       <c r="E25" t="n">
-        <v>38366952.15</v>
+        <v>11229431.75</v>
       </c>
       <c r="F25" t="n">
-        <v>22.216</v>
+        <v>-0.977</v>
       </c>
       <c r="G25" t="n">
-        <v>1.88416614</v>
+        <v>6.24965599</v>
       </c>
     </row>
     <row r="26">
@@ -1142,46 +1142,46 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.2333</v>
+        <v>0.239</v>
       </c>
       <c r="D26" t="n">
-        <v>65221490.0797</v>
+        <v>66168023.8557</v>
       </c>
       <c r="E26" t="n">
-        <v>279560609</v>
+        <v>276853656.3</v>
       </c>
       <c r="F26" t="n">
-        <v>17.828</v>
+        <v>19.381</v>
       </c>
       <c r="G26" t="n">
-        <v>0.25213359</v>
+        <v>0.2532168</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Aptos</t>
+          <t>THORChain</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>APT</t>
+          <t>RUNE</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>6.14</v>
+        <v>1.401</v>
       </c>
       <c r="D27" t="n">
-        <v>68553734.876</v>
+        <v>68714880.0636</v>
       </c>
       <c r="E27" t="n">
-        <v>11165103.4</v>
+        <v>49047023.6</v>
       </c>
       <c r="F27" t="n">
-        <v>-1.76</v>
+        <v>1.228</v>
       </c>
       <c r="G27" t="n">
-        <v>6.25470435</v>
+        <v>1.41607696</v>
       </c>
     </row>
     <row r="28">
@@ -1196,19 +1196,19 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>19.44</v>
+        <v>19.38</v>
       </c>
       <c r="D28" t="n">
-        <v>68061559.5432</v>
+        <v>67234017.51899999</v>
       </c>
       <c r="E28" t="n">
-        <v>3501109.03</v>
+        <v>3469247.55</v>
       </c>
       <c r="F28" t="n">
-        <v>3.957</v>
+        <v>4.026</v>
       </c>
       <c r="G28" t="n">
-        <v>19.13545324</v>
+        <v>19.15883459</v>
       </c>
     </row>
     <row r="29">
@@ -1223,19 +1223,19 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.24082</v>
+        <v>0.24018</v>
       </c>
       <c r="D29" t="n">
-        <v>64804298.3618</v>
+        <v>65921330.3448</v>
       </c>
       <c r="E29" t="n">
-        <v>269098490</v>
+        <v>274466360</v>
       </c>
       <c r="F29" t="n">
-        <v>1.321</v>
+        <v>1.44</v>
       </c>
       <c r="G29" t="n">
-        <v>0.23927207</v>
+        <v>0.23936172</v>
       </c>
     </row>
     <row r="30">
@@ -1250,19 +1250,19 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.2662</v>
+        <v>0.2645</v>
       </c>
       <c r="D30" t="n">
-        <v>60984090.6169</v>
+        <v>61744974.50585001</v>
       </c>
       <c r="E30" t="n">
-        <v>229091249.5</v>
+        <v>233440357.3</v>
       </c>
       <c r="F30" t="n">
-        <v>50.056</v>
+        <v>49.774</v>
       </c>
       <c r="G30" t="n">
-        <v>0.26517366</v>
+        <v>0.26524064</v>
       </c>
     </row>
     <row r="31">
@@ -1277,73 +1277,73 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.668</v>
+        <v>0.657</v>
       </c>
       <c r="D31" t="n">
-        <v>55813884.61264001</v>
+        <v>56550517.72866</v>
       </c>
       <c r="E31" t="n">
-        <v>83553719.48</v>
+        <v>86073847.38</v>
       </c>
       <c r="F31" t="n">
-        <v>2.297</v>
+        <v>-0.152</v>
       </c>
       <c r="G31" t="n">
-        <v>0.67383634</v>
+        <v>0.67329129</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>MANTRA</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>AAVE</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>5.9837</v>
+        <v>255.37</v>
       </c>
       <c r="D32" t="n">
-        <v>53247378.5706</v>
+        <v>54302407.71423</v>
       </c>
       <c r="E32" t="n">
-        <v>8898738</v>
+        <v>212642.079</v>
       </c>
       <c r="F32" t="n">
-        <v>-3.529</v>
+        <v>3.13</v>
       </c>
       <c r="G32" t="n">
-        <v>6.0547271</v>
+        <v>255.94602405</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>MANTRA</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>AAVE</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>258.62</v>
+        <v>5.9791</v>
       </c>
       <c r="D33" t="n">
-        <v>52434160.95106</v>
+        <v>51369909.9989</v>
       </c>
       <c r="E33" t="n">
-        <v>202745.963</v>
+        <v>8591579</v>
       </c>
       <c r="F33" t="n">
-        <v>4.093</v>
+        <v>-2.9</v>
       </c>
       <c r="G33" t="n">
-        <v>255.51102313</v>
+        <v>6.0390153</v>
       </c>
     </row>
     <row r="34">
@@ -1358,73 +1358,73 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.167</v>
+        <v>0.1609</v>
       </c>
       <c r="D34" t="n">
-        <v>48445170.91460001</v>
+        <v>48194222.37509999</v>
       </c>
       <c r="E34" t="n">
-        <v>290090843.8</v>
+        <v>299529039</v>
       </c>
       <c r="F34" t="n">
-        <v>0.602</v>
+        <v>-2.838</v>
       </c>
       <c r="G34" t="n">
-        <v>0.17253712</v>
+        <v>0.17213671</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Meld Bridged AVAX (Meld)</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>NEAR</t>
+          <t>AVAX</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3.359</v>
+        <v>26.36</v>
       </c>
       <c r="D35" t="n">
-        <v>49103858.2537</v>
+        <v>48034086.922</v>
       </c>
       <c r="E35" t="n">
-        <v>14618594.3</v>
+        <v>1822233.95</v>
       </c>
       <c r="F35" t="n">
-        <v>3.769</v>
+        <v>4.272</v>
       </c>
       <c r="G35" t="n">
-        <v>3.25561128</v>
+        <v>26.04792904</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Meld Bridged AVAX (Meld)</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>AVAX</t>
+          <t>NEAR</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>26.46</v>
+        <v>3.351</v>
       </c>
       <c r="D36" t="n">
-        <v>47864771.2242</v>
+        <v>48764044.2072</v>
       </c>
       <c r="E36" t="n">
-        <v>1808948.27</v>
+        <v>14552087.2</v>
       </c>
       <c r="F36" t="n">
-        <v>4.009</v>
+        <v>4.165</v>
       </c>
       <c r="G36" t="n">
-        <v>26.00875233</v>
+        <v>3.26008629</v>
       </c>
     </row>
     <row r="37">
@@ -1439,19 +1439,19 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>5.066</v>
+        <v>5.046</v>
       </c>
       <c r="D37" t="n">
-        <v>39853402.0679</v>
+        <v>40137826.91184</v>
       </c>
       <c r="E37" t="n">
-        <v>7866838.15</v>
+        <v>7954385.04</v>
       </c>
       <c r="F37" t="n">
-        <v>5.038</v>
+        <v>5.081</v>
       </c>
       <c r="G37" t="n">
-        <v>4.98037114</v>
+        <v>4.98821585</v>
       </c>
     </row>
     <row r="38">
@@ -1466,73 +1466,73 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.3326</v>
+        <v>0.3319</v>
       </c>
       <c r="D38" t="n">
-        <v>38696212.6296</v>
+        <v>37657550.2389</v>
       </c>
       <c r="E38" t="n">
-        <v>116344596</v>
+        <v>113460531</v>
       </c>
       <c r="F38" t="n">
-        <v>5.22</v>
+        <v>5.432</v>
       </c>
       <c r="G38" t="n">
-        <v>0.32319753</v>
+        <v>0.32373517</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Curve DAO</t>
+          <t>Raydium</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>CRV</t>
+          <t>RAY</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.5774</v>
+        <v>5.571</v>
       </c>
       <c r="D39" t="n">
-        <v>37911261.60918</v>
+        <v>38169919.3122</v>
       </c>
       <c r="E39" t="n">
-        <v>65658575.7</v>
+        <v>6851538.2</v>
       </c>
       <c r="F39" t="n">
-        <v>8.901999999999999</v>
+        <v>14.16</v>
       </c>
       <c r="G39" t="n">
-        <v>0.55761163</v>
+        <v>5.33245647</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Raydium</t>
+          <t>Curve DAO</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>RAY</t>
+          <t>CRV</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>5.616</v>
+        <v>0.5729</v>
       </c>
       <c r="D40" t="n">
-        <v>38452520.6208</v>
+        <v>37010394.65160999</v>
       </c>
       <c r="E40" t="n">
-        <v>6846958.8</v>
+        <v>64601840.9</v>
       </c>
       <c r="F40" t="n">
-        <v>15.556</v>
+        <v>9.52</v>
       </c>
       <c r="G40" t="n">
-        <v>5.30869872</v>
+        <v>0.55912403</v>
       </c>
     </row>
     <row r="41">
@@ -1547,73 +1547,73 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>9.935</v>
+        <v>9.819000000000001</v>
       </c>
       <c r="D41" t="n">
-        <v>36205940.37845001</v>
+        <v>36517724.18829001</v>
       </c>
       <c r="E41" t="n">
-        <v>3644281.87</v>
+        <v>3719087.91</v>
       </c>
       <c r="F41" t="n">
-        <v>8.579000000000001</v>
+        <v>7.558</v>
       </c>
       <c r="G41" t="n">
-        <v>9.60867043</v>
+        <v>9.62897315</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Arkham</t>
+          <t>Linea Bridged LDO (Linea)</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ARKM</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.712</v>
+        <v>1.62</v>
       </c>
       <c r="D42" t="n">
-        <v>35147053.012</v>
+        <v>35165634.9534</v>
       </c>
       <c r="E42" t="n">
-        <v>49363838.5</v>
+        <v>21707182.07</v>
       </c>
       <c r="F42" t="n">
-        <v>7.391</v>
+        <v>6.649</v>
       </c>
       <c r="G42" t="n">
-        <v>0.6822219</v>
+        <v>1.61161134</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Linea Bridged LDO (Linea)</t>
+          <t>Arkham</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>ARKM</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1.64</v>
+        <v>0.707</v>
       </c>
       <c r="D43" t="n">
-        <v>34055559.6624</v>
+        <v>35051478.2996</v>
       </c>
       <c r="E43" t="n">
-        <v>20765585.16</v>
+        <v>49577762.8</v>
       </c>
       <c r="F43" t="n">
-        <v>7.753</v>
+        <v>6.476</v>
       </c>
       <c r="G43" t="n">
-        <v>1.60890861</v>
+        <v>0.68386333</v>
       </c>
     </row>
     <row r="44">
@@ -1628,19 +1628,19 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.264</v>
+        <v>0.2604</v>
       </c>
       <c r="D44" t="n">
-        <v>32491872.0984</v>
+        <v>31725405.642</v>
       </c>
       <c r="E44" t="n">
-        <v>123075273.1</v>
+        <v>121833355</v>
       </c>
       <c r="F44" t="n">
-        <v>6.067</v>
+        <v>3.952</v>
       </c>
       <c r="G44" t="n">
-        <v>0.26358796</v>
+        <v>0.26390724</v>
       </c>
     </row>
     <row r="45">
@@ -1655,19 +1655,19 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.4684</v>
+        <v>0.4636</v>
       </c>
       <c r="D45" t="n">
-        <v>33045397.46316</v>
+        <v>31921531.12412</v>
       </c>
       <c r="E45" t="n">
-        <v>70549524.90000001</v>
+        <v>68855761.7</v>
       </c>
       <c r="F45" t="n">
-        <v>13.552</v>
+        <v>10.724</v>
       </c>
       <c r="G45" t="n">
-        <v>0.44346203</v>
+        <v>0.4457067</v>
       </c>
     </row>
     <row r="46">
@@ -1682,19 +1682,19 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.801</v>
+        <v>0.798</v>
       </c>
       <c r="D46" t="n">
-        <v>30195815.1669</v>
+        <v>29928895.038</v>
       </c>
       <c r="E46" t="n">
-        <v>37697646.9</v>
+        <v>37504881</v>
       </c>
       <c r="F46" t="n">
-        <v>2.824</v>
+        <v>2.439</v>
       </c>
       <c r="G46" t="n">
-        <v>0.79193766</v>
+        <v>0.79236586</v>
       </c>
     </row>
     <row r="47">
@@ -1709,46 +1709,46 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>9.823e-05</v>
+        <v>9.725000000000001e-05</v>
       </c>
       <c r="D47" t="n">
-        <v>29971067.7311111</v>
+        <v>29563992.3131655</v>
       </c>
       <c r="E47" t="n">
-        <v>305111144570</v>
+        <v>303999920958</v>
       </c>
       <c r="F47" t="n">
-        <v>4.456</v>
+        <v>3.689</v>
       </c>
       <c r="G47" t="n">
-        <v>9.676e-05</v>
+        <v>9.692e-05</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Magic Eden</t>
+          <t>Strategic Hub for Innovation in Blockchain</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ME</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1.897</v>
+        <v>1.604e-05</v>
       </c>
       <c r="D48" t="n">
-        <v>30172712.0639</v>
+        <v>28923325.20721144</v>
       </c>
       <c r="E48" t="n">
-        <v>15905488.7</v>
+        <v>1803199825886</v>
       </c>
       <c r="F48" t="n">
-        <v>4.231</v>
+        <v>1.777</v>
       </c>
       <c r="G48" t="n">
-        <v>1.85221751</v>
+        <v>1.607e-05</v>
       </c>
     </row>
     <row r="49">
@@ -1763,73 +1763,73 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.01596</v>
+        <v>0.01597</v>
       </c>
       <c r="D49" t="n">
-        <v>27540257.24688</v>
+        <v>27633807.05517</v>
       </c>
       <c r="E49" t="n">
-        <v>1725580028</v>
+        <v>1730357361</v>
       </c>
       <c r="F49" t="n">
-        <v>21.369</v>
+        <v>21.537</v>
       </c>
       <c r="G49" t="n">
-        <v>0.01661577</v>
+        <v>0.0166497</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Strategic Hub for Innovation in Blockchain</t>
+          <t>Magic Eden</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>ME</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1.614e-05</v>
+        <v>1.871</v>
       </c>
       <c r="D50" t="n">
-        <v>27849761.28677694</v>
+        <v>28711238.66637</v>
       </c>
       <c r="E50" t="n">
-        <v>1725511851721</v>
+        <v>15345397.47</v>
       </c>
       <c r="F50" t="n">
-        <v>1.765</v>
+        <v>3.142</v>
       </c>
       <c r="G50" t="n">
-        <v>1.606e-05</v>
+        <v>1.85567692</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>Rocket Pool</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>RPL</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>3.449</v>
+        <v>11.38</v>
       </c>
       <c r="D51" t="n">
-        <v>28320306.11907</v>
+        <v>30789149.4408</v>
       </c>
       <c r="E51" t="n">
-        <v>8211164.43</v>
+        <v>2705549.16</v>
       </c>
       <c r="F51" t="n">
-        <v>8.289</v>
+        <v>51.129</v>
       </c>
       <c r="G51" t="n">
-        <v>3.36497328</v>
+        <v>10.3128274</v>
       </c>
     </row>
   </sheetData>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>2025-02-11 16:55</t>
+          <t>2025-02-11 18:05</t>
         </is>
       </c>
     </row>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$9,445,967,756.50</t>
+          <t>$9,490,989,624.88</t>
         </is>
       </c>
     </row>
@@ -1891,7 +1891,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>$22,980,366,673,760.23</t>
+          <t>$23,657,869,021,964.33</t>
         </is>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$2,051.47</t>
+          <t>$2,043.88</t>
         </is>
       </c>
     </row>
@@ -1926,7 +1926,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9">
@@ -1936,7 +1936,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>